<commit_message>
Actualizando cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Documentos/Planes/SRGAS-CP.xlsx
+++ b/Documentos/Planes/SRGAS-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Escritorio\ProyectoGimnasio\ProyectoGimnasio\Documentos\Planes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F156E6E-1987-499C-8087-F6099D20B0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D6D46A-6B41-4487-8D4F-5F74AA34D1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,13 +516,13 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -757,26 +757,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
@@ -792,22 +792,22 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1315,7 +1315,7 @@
       <c r="G28" s="15">
         <v>45186</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H28" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       <c r="G42" s="15">
         <v>45214</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
         <v>45229</v>
       </c>
       <c r="H57" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2000,7 +2000,7 @@
         <v>45229</v>
       </c>
       <c r="H58" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
         <v>45229</v>
       </c>
       <c r="H59" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>